<commit_message>
testing a different 2D scheme
</commit_message>
<xml_diff>
--- a/Figs/DF_results_test.xlsx
+++ b/Figs/DF_results_test.xlsx
@@ -17,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <name val="Aptos Narrow"/>
       <family val="2"/>
@@ -29,6 +29,12 @@
       <name val="Aptos Narrow"/>
       <b val="1"/>
       <sz val="12"/>
+    </font>
+    <font>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <sz val="8"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -66,15 +72,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
@@ -468,10 +487,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J40"/>
+  <dimension ref="A1:J43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -829,32 +848,32 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.04082895579827373</v>
+        <v>0.0393554853922049</v>
       </c>
       <c r="C11" t="n">
-        <v>0.0106411895144973</v>
+        <v>0.010819523336726</v>
       </c>
       <c r="D11" t="n">
-        <v>0.01740590862918504</v>
+        <v>0.01715549444968637</v>
       </c>
       <c r="E11" t="n">
-        <v>0.04082895579827373</v>
+        <v>0.0393554853922049</v>
       </c>
       <c r="F11" t="n">
-        <v>0.0106411895144973</v>
+        <v>0.010819523336726</v>
       </c>
       <c r="G11" t="n">
-        <v>0.01740590862918504</v>
+        <v>0.01715549444968637</v>
       </c>
       <c r="H11" t="n">
-        <v>0.0322868824005127</v>
+        <v>0.04361820220947266</v>
       </c>
       <c r="I11" t="n">
         <v>0.5</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>Changing floating point precision of second derivative to float16</t>
+          <t>Setting second derivative to 0</t>
         </is>
       </c>
     </row>
@@ -865,32 +884,32 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.0408288836479187</v>
+        <v>0.03935545682907104</v>
       </c>
       <c r="C12" t="n">
-        <v>0.01064119301736355</v>
+        <v>0.01081951148808002</v>
       </c>
       <c r="D12" t="n">
-        <v>0.01740591786801815</v>
+        <v>0.0171554908156395</v>
       </c>
       <c r="E12" t="n">
-        <v>0.0408288836479187</v>
+        <v>0.03935545682907104</v>
       </c>
       <c r="F12" t="n">
-        <v>0.01064119301736355</v>
+        <v>0.01081951148808002</v>
       </c>
       <c r="G12" t="n">
-        <v>0.01740591786801815</v>
+        <v>0.0171554908156395</v>
       </c>
       <c r="H12" t="n">
-        <v>0.02213692665100098</v>
+        <v>0.01541471481323242</v>
       </c>
       <c r="I12" t="n">
         <v>0.5</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>Changing floating point precision of second derivative to float16</t>
+          <t>Setting second derivative to 0</t>
         </is>
       </c>
     </row>
@@ -904,29 +923,29 @@
         <v>0.041015625</v>
       </c>
       <c r="C13" t="n">
-        <v>0.0110321044921875</v>
+        <v>0.010711669921875</v>
       </c>
       <c r="D13" t="n">
-        <v>0.0175933837890625</v>
+        <v>0.0171661376953125</v>
       </c>
       <c r="E13" t="n">
         <v>0.041015625</v>
       </c>
       <c r="F13" t="n">
-        <v>0.0110321044921875</v>
+        <v>0.010711669921875</v>
       </c>
       <c r="G13" t="n">
-        <v>0.0175933837890625</v>
+        <v>0.0171661376953125</v>
       </c>
       <c r="H13" t="n">
-        <v>0.1135258674621582</v>
+        <v>0.1023433208465576</v>
       </c>
       <c r="I13" t="n">
         <v>0.5</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>Changing floating point precision of second derivative to float16</t>
+          <t>Setting second derivative to 0</t>
         </is>
       </c>
     </row>
@@ -937,32 +956,32 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.0393554853922049</v>
+        <v>0.04082895579827373</v>
       </c>
       <c r="C14" t="n">
-        <v>0.010819523336726</v>
+        <v>0.0106411895144973</v>
       </c>
       <c r="D14" t="n">
-        <v>0.01715549444968637</v>
+        <v>0.01740590862918504</v>
       </c>
       <c r="E14" t="n">
-        <v>0.0393554853922049</v>
+        <v>0.04082895579827373</v>
       </c>
       <c r="F14" t="n">
-        <v>0.010819523336726</v>
+        <v>0.0106411895144973</v>
       </c>
       <c r="G14" t="n">
-        <v>0.01715549444968637</v>
+        <v>0.01740590862918504</v>
       </c>
       <c r="H14" t="n">
-        <v>0.04361820220947266</v>
+        <v>0.0322868824005127</v>
       </c>
       <c r="I14" t="n">
         <v>0.5</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>Setting second derivative to 0</t>
+          <t>Setting the second derivative precision to float16</t>
         </is>
       </c>
     </row>
@@ -973,32 +992,32 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.03935545682907104</v>
+        <v>0.0408288836479187</v>
       </c>
       <c r="C15" t="n">
-        <v>0.01081951148808002</v>
+        <v>0.01064119301736355</v>
       </c>
       <c r="D15" t="n">
-        <v>0.0171554908156395</v>
+        <v>0.01740591786801815</v>
       </c>
       <c r="E15" t="n">
-        <v>0.03935545682907104</v>
+        <v>0.0408288836479187</v>
       </c>
       <c r="F15" t="n">
-        <v>0.01081951148808002</v>
+        <v>0.01064119301736355</v>
       </c>
       <c r="G15" t="n">
-        <v>0.0171554908156395</v>
+        <v>0.01740591786801815</v>
       </c>
       <c r="H15" t="n">
-        <v>0.01541471481323242</v>
+        <v>0.02213692665100098</v>
       </c>
       <c r="I15" t="n">
         <v>0.5</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>Setting second derivative to 0</t>
+          <t>Setting the second derivative precision to float16</t>
         </is>
       </c>
     </row>
@@ -1012,29 +1031,29 @@
         <v>0.041015625</v>
       </c>
       <c r="C16" t="n">
-        <v>0.010711669921875</v>
+        <v>0.0110321044921875</v>
       </c>
       <c r="D16" t="n">
-        <v>0.0171661376953125</v>
+        <v>0.0175933837890625</v>
       </c>
       <c r="E16" t="n">
         <v>0.041015625</v>
       </c>
       <c r="F16" t="n">
-        <v>0.010711669921875</v>
+        <v>0.0110321044921875</v>
       </c>
       <c r="G16" t="n">
-        <v>0.0171661376953125</v>
+        <v>0.0175933837890625</v>
       </c>
       <c r="H16" t="n">
-        <v>0.1023433208465576</v>
+        <v>0.1135258674621582</v>
       </c>
       <c r="I16" t="n">
         <v>0.5</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>Setting second derivative to 0</t>
+          <t>Setting the second derivative precision to float16</t>
         </is>
       </c>
     </row>
@@ -1902,7 +1921,120 @@
         </is>
       </c>
     </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>float64</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>0.1276876932869065</v>
+      </c>
+      <c r="C41" t="n">
+        <v>0.04101136420033664</v>
+      </c>
+      <c r="D41" t="n">
+        <v>0.05986374395391551</v>
+      </c>
+      <c r="E41" t="n">
+        <v>0.1276876932869065</v>
+      </c>
+      <c r="F41" t="n">
+        <v>0.04101136420033664</v>
+      </c>
+      <c r="G41" t="n">
+        <v>0.05986374395391551</v>
+      </c>
+      <c r="H41" t="n">
+        <v>0.1105630397796631</v>
+      </c>
+      <c r="I41" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>float32</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>0.1276876926422119</v>
+      </c>
+      <c r="C42" t="n">
+        <v>0.04101136326789856</v>
+      </c>
+      <c r="D42" t="n">
+        <v>0.05986374616622925</v>
+      </c>
+      <c r="E42" t="n">
+        <v>0.1276876926422119</v>
+      </c>
+      <c r="F42" t="n">
+        <v>0.04101136326789856</v>
+      </c>
+      <c r="G42" t="n">
+        <v>0.05986374616622925</v>
+      </c>
+      <c r="H42" t="n">
+        <v>0.0634009838104248</v>
+      </c>
+      <c r="I42" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="J42" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>float16</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>0.12841796875</v>
+      </c>
+      <c r="C43" t="n">
+        <v>0.041046142578125</v>
+      </c>
+      <c r="D43" t="n">
+        <v>0.059539794921875</v>
+      </c>
+      <c r="E43" t="n">
+        <v>0.12841796875</v>
+      </c>
+      <c r="F43" t="n">
+        <v>0.041046142578125</v>
+      </c>
+      <c r="G43" t="n">
+        <v>0.059539794921875</v>
+      </c>
+      <c r="H43" t="n">
+        <v>0.5770299434661865</v>
+      </c>
+      <c r="I43" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="J43" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="C2">
+    <cfRule type="expression" priority="1" dxfId="0">
+      <formula>AND(A4="float16", OR(B4&lt;B3, B4&lt;B2))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>